<commit_message>
fixed formatting for position graph
</commit_message>
<xml_diff>
--- a/reddit_data.xlsx
+++ b/reddit_data.xlsx
@@ -1,16 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23328"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Visual Studio Code Workspace\WSB Scraper\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56839760-FEAF-457E-B25B-2C5563949C67}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="58965" yWindow="9435" windowWidth="24615" windowHeight="12285" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -347,71 +353,71 @@
     <t>FSLY</t>
   </si>
   <si>
-    <t>ACB 12/11 7p</t>
-  </si>
-  <si>
-    <t>CRSR 12/18 45C</t>
-  </si>
-  <si>
-    <t>F 12/4 10c</t>
-  </si>
-  <si>
-    <t>FB 12/18 300c</t>
-  </si>
-  <si>
-    <t>FB 12/4 290C</t>
-  </si>
-  <si>
-    <t>FSLY 12/4 90C</t>
-  </si>
-  <si>
-    <t>GME 12/18 20C</t>
-  </si>
-  <si>
-    <t>NKLA 12/31 20P</t>
-  </si>
-  <si>
-    <t>NKLA 12/4 17p</t>
-  </si>
-  <si>
-    <t>PLTR 1/15 40c</t>
-  </si>
-  <si>
-    <t>PLTR 12/31 32c</t>
-  </si>
-  <si>
-    <t>PLTR 12/31 35C</t>
-  </si>
-  <si>
-    <t>PLTR 12/4 35c</t>
-  </si>
-  <si>
-    <t>PLTR 12/4 38c</t>
-  </si>
-  <si>
-    <t>SLV 12/18 25c</t>
-  </si>
-  <si>
-    <t>SNOW 12/18 365c</t>
-  </si>
-  <si>
-    <t>SPY 12/4 362p</t>
-  </si>
-  <si>
-    <t>TSLA 12/11 600c</t>
-  </si>
-  <si>
-    <t>TSLA 12/4 650c</t>
-  </si>
-  <si>
-    <t>TSM 1/21 80c</t>
+    <t>12/11 7p</t>
+  </si>
+  <si>
+    <t>12/18 45C</t>
+  </si>
+  <si>
+    <t>12/4 10c</t>
+  </si>
+  <si>
+    <t>12/18 300c</t>
+  </si>
+  <si>
+    <t>12/4 290C</t>
+  </si>
+  <si>
+    <t>12/4 90C</t>
+  </si>
+  <si>
+    <t>12/18 20C</t>
+  </si>
+  <si>
+    <t>12/31 20P</t>
+  </si>
+  <si>
+    <t>12/4 17p</t>
+  </si>
+  <si>
+    <t>1/15 40c</t>
+  </si>
+  <si>
+    <t>12/31 32c</t>
+  </si>
+  <si>
+    <t>12/31 35C</t>
+  </si>
+  <si>
+    <t>12/4 35c</t>
+  </si>
+  <si>
+    <t>12/4 38c</t>
+  </si>
+  <si>
+    <t>12/18 25c</t>
+  </si>
+  <si>
+    <t>12/18 365c</t>
+  </si>
+  <si>
+    <t>12/4 362p</t>
+  </si>
+  <si>
+    <t>12/11 600c</t>
+  </si>
+  <si>
+    <t>12/4 650c</t>
+  </si>
+  <si>
+    <t>1/21 80c</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -463,8 +469,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -474,25 +483,737 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
   <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:barChart>
         <c:barDir val="col"/>
         <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
+          <c:invertIfNegative val="0"/>
           <c:cat>
-            <c:numRef>
-              <c:f>Sheet1!$B$2:$A$125</c:f>
-            </c:numRef>
+            <c:multiLvlStrRef>
+              <c:f>Sheet1!$A$2:$B$125</c:f>
+              <c:multiLvlStrCache>
+                <c:ptCount val="124"/>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>calls</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>puts</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>calls</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>puts</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>calls</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>puts</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>calls</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>calls</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>calls</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>calls</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>calls</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
+                    <c:v>calls</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>calls</c:v>
+                  </c:pt>
+                  <c:pt idx="13">
+                    <c:v>calls</c:v>
+                  </c:pt>
+                  <c:pt idx="14">
+                    <c:v>calls</c:v>
+                  </c:pt>
+                  <c:pt idx="15">
+                    <c:v>calls</c:v>
+                  </c:pt>
+                  <c:pt idx="16">
+                    <c:v>calls</c:v>
+                  </c:pt>
+                  <c:pt idx="17">
+                    <c:v>puts</c:v>
+                  </c:pt>
+                  <c:pt idx="18">
+                    <c:v>calls</c:v>
+                  </c:pt>
+                  <c:pt idx="19">
+                    <c:v>calls</c:v>
+                  </c:pt>
+                  <c:pt idx="20">
+                    <c:v>calls</c:v>
+                  </c:pt>
+                  <c:pt idx="21">
+                    <c:v>calls</c:v>
+                  </c:pt>
+                  <c:pt idx="22">
+                    <c:v>calls</c:v>
+                  </c:pt>
+                  <c:pt idx="23">
+                    <c:v>calls</c:v>
+                  </c:pt>
+                  <c:pt idx="24">
+                    <c:v>calls</c:v>
+                  </c:pt>
+                  <c:pt idx="25">
+                    <c:v>calls</c:v>
+                  </c:pt>
+                  <c:pt idx="26">
+                    <c:v>calls</c:v>
+                  </c:pt>
+                  <c:pt idx="27">
+                    <c:v>calls</c:v>
+                  </c:pt>
+                  <c:pt idx="28">
+                    <c:v>calls</c:v>
+                  </c:pt>
+                  <c:pt idx="29">
+                    <c:v>puts</c:v>
+                  </c:pt>
+                  <c:pt idx="30">
+                    <c:v>calls</c:v>
+                  </c:pt>
+                  <c:pt idx="31">
+                    <c:v>calls</c:v>
+                  </c:pt>
+                  <c:pt idx="32">
+                    <c:v>calls</c:v>
+                  </c:pt>
+                  <c:pt idx="33">
+                    <c:v>calls</c:v>
+                  </c:pt>
+                  <c:pt idx="34">
+                    <c:v>calls</c:v>
+                  </c:pt>
+                  <c:pt idx="35">
+                    <c:v>calls</c:v>
+                  </c:pt>
+                  <c:pt idx="36">
+                    <c:v>puts</c:v>
+                  </c:pt>
+                  <c:pt idx="37">
+                    <c:v>calls</c:v>
+                  </c:pt>
+                  <c:pt idx="38">
+                    <c:v>calls</c:v>
+                  </c:pt>
+                  <c:pt idx="39">
+                    <c:v>calls</c:v>
+                  </c:pt>
+                  <c:pt idx="40">
+                    <c:v>calls</c:v>
+                  </c:pt>
+                  <c:pt idx="41">
+                    <c:v>puts</c:v>
+                  </c:pt>
+                  <c:pt idx="42">
+                    <c:v>calls</c:v>
+                  </c:pt>
+                  <c:pt idx="43">
+                    <c:v>puts</c:v>
+                  </c:pt>
+                  <c:pt idx="44">
+                    <c:v>calls</c:v>
+                  </c:pt>
+                  <c:pt idx="45">
+                    <c:v>calls</c:v>
+                  </c:pt>
+                  <c:pt idx="46">
+                    <c:v>calls</c:v>
+                  </c:pt>
+                  <c:pt idx="47">
+                    <c:v>calls</c:v>
+                  </c:pt>
+                  <c:pt idx="48">
+                    <c:v>puts</c:v>
+                  </c:pt>
+                  <c:pt idx="49">
+                    <c:v>calls</c:v>
+                  </c:pt>
+                  <c:pt idx="50">
+                    <c:v>calls</c:v>
+                  </c:pt>
+                  <c:pt idx="51">
+                    <c:v>calls</c:v>
+                  </c:pt>
+                  <c:pt idx="52">
+                    <c:v>puts</c:v>
+                  </c:pt>
+                  <c:pt idx="53">
+                    <c:v>calls</c:v>
+                  </c:pt>
+                  <c:pt idx="54">
+                    <c:v>calls</c:v>
+                  </c:pt>
+                  <c:pt idx="55">
+                    <c:v>puts</c:v>
+                  </c:pt>
+                  <c:pt idx="56">
+                    <c:v>calls</c:v>
+                  </c:pt>
+                  <c:pt idx="57">
+                    <c:v>puts</c:v>
+                  </c:pt>
+                  <c:pt idx="58">
+                    <c:v>puts</c:v>
+                  </c:pt>
+                  <c:pt idx="59">
+                    <c:v>calls</c:v>
+                  </c:pt>
+                  <c:pt idx="60">
+                    <c:v>puts</c:v>
+                  </c:pt>
+                  <c:pt idx="61">
+                    <c:v>calls</c:v>
+                  </c:pt>
+                  <c:pt idx="62">
+                    <c:v>calls</c:v>
+                  </c:pt>
+                  <c:pt idx="63">
+                    <c:v>puts</c:v>
+                  </c:pt>
+                  <c:pt idx="64">
+                    <c:v>calls</c:v>
+                  </c:pt>
+                  <c:pt idx="65">
+                    <c:v>calls</c:v>
+                  </c:pt>
+                  <c:pt idx="66">
+                    <c:v>calls</c:v>
+                  </c:pt>
+                  <c:pt idx="67">
+                    <c:v>calls</c:v>
+                  </c:pt>
+                  <c:pt idx="68">
+                    <c:v>puts</c:v>
+                  </c:pt>
+                  <c:pt idx="69">
+                    <c:v>calls</c:v>
+                  </c:pt>
+                  <c:pt idx="70">
+                    <c:v>calls</c:v>
+                  </c:pt>
+                  <c:pt idx="71">
+                    <c:v>calls</c:v>
+                  </c:pt>
+                  <c:pt idx="72">
+                    <c:v>calls</c:v>
+                  </c:pt>
+                  <c:pt idx="73">
+                    <c:v>puts</c:v>
+                  </c:pt>
+                  <c:pt idx="74">
+                    <c:v>calls</c:v>
+                  </c:pt>
+                  <c:pt idx="75">
+                    <c:v>puts</c:v>
+                  </c:pt>
+                  <c:pt idx="76">
+                    <c:v>calls</c:v>
+                  </c:pt>
+                  <c:pt idx="77">
+                    <c:v>calls</c:v>
+                  </c:pt>
+                  <c:pt idx="78">
+                    <c:v>puts</c:v>
+                  </c:pt>
+                  <c:pt idx="79">
+                    <c:v>calls</c:v>
+                  </c:pt>
+                  <c:pt idx="80">
+                    <c:v>calls</c:v>
+                  </c:pt>
+                  <c:pt idx="81">
+                    <c:v>puts</c:v>
+                  </c:pt>
+                  <c:pt idx="82">
+                    <c:v>calls</c:v>
+                  </c:pt>
+                  <c:pt idx="83">
+                    <c:v>calls</c:v>
+                  </c:pt>
+                  <c:pt idx="84">
+                    <c:v>calls</c:v>
+                  </c:pt>
+                  <c:pt idx="85">
+                    <c:v>calls</c:v>
+                  </c:pt>
+                  <c:pt idx="86">
+                    <c:v>calls</c:v>
+                  </c:pt>
+                  <c:pt idx="87">
+                    <c:v>puts</c:v>
+                  </c:pt>
+                  <c:pt idx="88">
+                    <c:v>calls</c:v>
+                  </c:pt>
+                  <c:pt idx="89">
+                    <c:v>calls</c:v>
+                  </c:pt>
+                  <c:pt idx="90">
+                    <c:v>puts</c:v>
+                  </c:pt>
+                  <c:pt idx="91">
+                    <c:v>calls</c:v>
+                  </c:pt>
+                  <c:pt idx="92">
+                    <c:v>calls</c:v>
+                  </c:pt>
+                  <c:pt idx="93">
+                    <c:v>calls</c:v>
+                  </c:pt>
+                  <c:pt idx="94">
+                    <c:v>calls</c:v>
+                  </c:pt>
+                  <c:pt idx="95">
+                    <c:v>calls</c:v>
+                  </c:pt>
+                  <c:pt idx="96">
+                    <c:v>calls</c:v>
+                  </c:pt>
+                  <c:pt idx="97">
+                    <c:v>calls</c:v>
+                  </c:pt>
+                  <c:pt idx="98">
+                    <c:v>calls</c:v>
+                  </c:pt>
+                  <c:pt idx="99">
+                    <c:v>puts</c:v>
+                  </c:pt>
+                  <c:pt idx="100">
+                    <c:v>calls</c:v>
+                  </c:pt>
+                  <c:pt idx="101">
+                    <c:v>calls</c:v>
+                  </c:pt>
+                  <c:pt idx="102">
+                    <c:v>calls</c:v>
+                  </c:pt>
+                  <c:pt idx="103">
+                    <c:v>calls</c:v>
+                  </c:pt>
+                  <c:pt idx="104">
+                    <c:v>calls</c:v>
+                  </c:pt>
+                  <c:pt idx="105">
+                    <c:v>puts</c:v>
+                  </c:pt>
+                  <c:pt idx="106">
+                    <c:v>calls</c:v>
+                  </c:pt>
+                  <c:pt idx="107">
+                    <c:v>calls</c:v>
+                  </c:pt>
+                  <c:pt idx="108">
+                    <c:v>calls</c:v>
+                  </c:pt>
+                  <c:pt idx="109">
+                    <c:v>calls</c:v>
+                  </c:pt>
+                  <c:pt idx="110">
+                    <c:v>calls</c:v>
+                  </c:pt>
+                  <c:pt idx="111">
+                    <c:v>calls</c:v>
+                  </c:pt>
+                  <c:pt idx="112">
+                    <c:v>calls</c:v>
+                  </c:pt>
+                  <c:pt idx="113">
+                    <c:v>calls</c:v>
+                  </c:pt>
+                  <c:pt idx="114">
+                    <c:v>calls</c:v>
+                  </c:pt>
+                  <c:pt idx="115">
+                    <c:v>calls</c:v>
+                  </c:pt>
+                  <c:pt idx="116">
+                    <c:v>calls</c:v>
+                  </c:pt>
+                  <c:pt idx="117">
+                    <c:v>calls</c:v>
+                  </c:pt>
+                  <c:pt idx="118">
+                    <c:v>puts</c:v>
+                  </c:pt>
+                  <c:pt idx="119">
+                    <c:v>calls</c:v>
+                  </c:pt>
+                  <c:pt idx="120">
+                    <c:v>calls</c:v>
+                  </c:pt>
+                  <c:pt idx="121">
+                    <c:v>puts</c:v>
+                  </c:pt>
+                  <c:pt idx="122">
+                    <c:v>calls</c:v>
+                  </c:pt>
+                  <c:pt idx="123">
+                    <c:v>puts</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>AAL</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>AAPL</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>AARK</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>ACB</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>AMD</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>AMZN</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>AND</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>AOL</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>APHA</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
+                    <c:v>APPL</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>ASML</c:v>
+                  </c:pt>
+                  <c:pt idx="13">
+                    <c:v>ATM</c:v>
+                  </c:pt>
+                  <c:pt idx="14">
+                    <c:v>BA</c:v>
+                  </c:pt>
+                  <c:pt idx="15">
+                    <c:v>BABA</c:v>
+                  </c:pt>
+                  <c:pt idx="16">
+                    <c:v>BB</c:v>
+                  </c:pt>
+                  <c:pt idx="18">
+                    <c:v>BBY</c:v>
+                  </c:pt>
+                  <c:pt idx="19">
+                    <c:v>BNTX</c:v>
+                  </c:pt>
+                  <c:pt idx="20">
+                    <c:v>BP</c:v>
+                  </c:pt>
+                  <c:pt idx="21">
+                    <c:v>CAAS</c:v>
+                  </c:pt>
+                  <c:pt idx="22">
+                    <c:v>CGC</c:v>
+                  </c:pt>
+                  <c:pt idx="23">
+                    <c:v>CHEWY</c:v>
+                  </c:pt>
+                  <c:pt idx="24">
+                    <c:v>CHWY</c:v>
+                  </c:pt>
+                  <c:pt idx="25">
+                    <c:v>CLF</c:v>
+                  </c:pt>
+                  <c:pt idx="26">
+                    <c:v>COST</c:v>
+                  </c:pt>
+                  <c:pt idx="27">
+                    <c:v>CRM</c:v>
+                  </c:pt>
+                  <c:pt idx="28">
+                    <c:v>CRSR</c:v>
+                  </c:pt>
+                  <c:pt idx="30">
+                    <c:v>CVS</c:v>
+                  </c:pt>
+                  <c:pt idx="31">
+                    <c:v>DG</c:v>
+                  </c:pt>
+                  <c:pt idx="32">
+                    <c:v>DIA</c:v>
+                  </c:pt>
+                  <c:pt idx="33">
+                    <c:v>DKNG</c:v>
+                  </c:pt>
+                  <c:pt idx="34">
+                    <c:v>DOTM</c:v>
+                  </c:pt>
+                  <c:pt idx="35">
+                    <c:v>DTE</c:v>
+                  </c:pt>
+                  <c:pt idx="37">
+                    <c:v>EOY</c:v>
+                  </c:pt>
+                  <c:pt idx="38">
+                    <c:v>ETSY</c:v>
+                  </c:pt>
+                  <c:pt idx="39">
+                    <c:v>EV</c:v>
+                  </c:pt>
+                  <c:pt idx="40">
+                    <c:v>FB</c:v>
+                  </c:pt>
+                  <c:pt idx="42">
+                    <c:v>FD</c:v>
+                  </c:pt>
+                  <c:pt idx="44">
+                    <c:v>FDX</c:v>
+                  </c:pt>
+                  <c:pt idx="45">
+                    <c:v>GDXJ</c:v>
+                  </c:pt>
+                  <c:pt idx="46">
+                    <c:v>GE</c:v>
+                  </c:pt>
+                  <c:pt idx="47">
+                    <c:v>GME</c:v>
+                  </c:pt>
+                  <c:pt idx="49">
+                    <c:v>HCACK</c:v>
+                  </c:pt>
+                  <c:pt idx="50">
+                    <c:v>HEXO</c:v>
+                  </c:pt>
+                  <c:pt idx="51">
+                    <c:v>I</c:v>
+                  </c:pt>
+                  <c:pt idx="53">
+                    <c:v>ICLN</c:v>
+                  </c:pt>
+                  <c:pt idx="54">
+                    <c:v>INTC</c:v>
+                  </c:pt>
+                  <c:pt idx="56">
+                    <c:v>ITM</c:v>
+                  </c:pt>
+                  <c:pt idx="58">
+                    <c:v>IV</c:v>
+                  </c:pt>
+                  <c:pt idx="59">
+                    <c:v>IWM</c:v>
+                  </c:pt>
+                  <c:pt idx="61">
+                    <c:v>JD</c:v>
+                  </c:pt>
+                  <c:pt idx="62">
+                    <c:v>JETS</c:v>
+                  </c:pt>
+                  <c:pt idx="63">
+                    <c:v>JMIA</c:v>
+                  </c:pt>
+                  <c:pt idx="64">
+                    <c:v>JNJ</c:v>
+                  </c:pt>
+                  <c:pt idx="65">
+                    <c:v>KR</c:v>
+                  </c:pt>
+                  <c:pt idx="66">
+                    <c:v>MJ</c:v>
+                  </c:pt>
+                  <c:pt idx="67">
+                    <c:v>MRNA</c:v>
+                  </c:pt>
+                  <c:pt idx="69">
+                    <c:v>MSFT</c:v>
+                  </c:pt>
+                  <c:pt idx="70">
+                    <c:v>MU</c:v>
+                  </c:pt>
+                  <c:pt idx="71">
+                    <c:v>NET</c:v>
+                  </c:pt>
+                  <c:pt idx="72">
+                    <c:v>NIO</c:v>
+                  </c:pt>
+                  <c:pt idx="74">
+                    <c:v>NKLA</c:v>
+                  </c:pt>
+                  <c:pt idx="76">
+                    <c:v>NOK</c:v>
+                  </c:pt>
+                  <c:pt idx="77">
+                    <c:v>OTM</c:v>
+                  </c:pt>
+                  <c:pt idx="79">
+                    <c:v>PFE</c:v>
+                  </c:pt>
+                  <c:pt idx="80">
+                    <c:v>PLTR</c:v>
+                  </c:pt>
+                  <c:pt idx="82">
+                    <c:v>PLUG</c:v>
+                  </c:pt>
+                  <c:pt idx="83">
+                    <c:v>PSTH</c:v>
+                  </c:pt>
+                  <c:pt idx="84">
+                    <c:v>PTLR</c:v>
+                  </c:pt>
+                  <c:pt idx="85">
+                    <c:v>PTON</c:v>
+                  </c:pt>
+                  <c:pt idx="86">
+                    <c:v>PTVE</c:v>
+                  </c:pt>
+                  <c:pt idx="87">
+                    <c:v>QQQ</c:v>
+                  </c:pt>
+                  <c:pt idx="88">
+                    <c:v>QQQJ</c:v>
+                  </c:pt>
+                  <c:pt idx="89">
+                    <c:v>RIOT</c:v>
+                  </c:pt>
+                  <c:pt idx="90">
+                    <c:v>RNA</c:v>
+                  </c:pt>
+                  <c:pt idx="91">
+                    <c:v>ROPE</c:v>
+                  </c:pt>
+                  <c:pt idx="92">
+                    <c:v>SHOP</c:v>
+                  </c:pt>
+                  <c:pt idx="93">
+                    <c:v>SLV</c:v>
+                  </c:pt>
+                  <c:pt idx="94">
+                    <c:v>SNE</c:v>
+                  </c:pt>
+                  <c:pt idx="95">
+                    <c:v>SNOW</c:v>
+                  </c:pt>
+                  <c:pt idx="96">
+                    <c:v>SPCE</c:v>
+                  </c:pt>
+                  <c:pt idx="97">
+                    <c:v>SPXS</c:v>
+                  </c:pt>
+                  <c:pt idx="98">
+                    <c:v>SPY</c:v>
+                  </c:pt>
+                  <c:pt idx="100">
+                    <c:v>STM</c:v>
+                  </c:pt>
+                  <c:pt idx="101">
+                    <c:v>TLRY</c:v>
+                  </c:pt>
+                  <c:pt idx="102">
+                    <c:v>TLSA</c:v>
+                  </c:pt>
+                  <c:pt idx="103">
+                    <c:v>TMO</c:v>
+                  </c:pt>
+                  <c:pt idx="104">
+                    <c:v>TSLA</c:v>
+                  </c:pt>
+                  <c:pt idx="106">
+                    <c:v>TSM</c:v>
+                  </c:pt>
+                  <c:pt idx="107">
+                    <c:v>TWM</c:v>
+                  </c:pt>
+                  <c:pt idx="108">
+                    <c:v>U</c:v>
+                  </c:pt>
+                  <c:pt idx="109">
+                    <c:v>UK</c:v>
+                  </c:pt>
+                  <c:pt idx="110">
+                    <c:v>UPS</c:v>
+                  </c:pt>
+                  <c:pt idx="111">
+                    <c:v>UVXY</c:v>
+                  </c:pt>
+                  <c:pt idx="112">
+                    <c:v>VALE</c:v>
+                  </c:pt>
+                  <c:pt idx="113">
+                    <c:v>VIX</c:v>
+                  </c:pt>
+                  <c:pt idx="114">
+                    <c:v>VRAM</c:v>
+                  </c:pt>
+                  <c:pt idx="115">
+                    <c:v>VXX</c:v>
+                  </c:pt>
+                  <c:pt idx="116">
+                    <c:v>WFC</c:v>
+                  </c:pt>
+                  <c:pt idx="117">
+                    <c:v>WORK</c:v>
+                  </c:pt>
+                  <c:pt idx="118">
+                    <c:v>WSB</c:v>
+                  </c:pt>
+                  <c:pt idx="119">
+                    <c:v>X</c:v>
+                  </c:pt>
+                  <c:pt idx="120">
+                    <c:v>XOM</c:v>
+                  </c:pt>
+                  <c:pt idx="121">
+                    <c:v>ZI</c:v>
+                  </c:pt>
+                  <c:pt idx="122">
+                    <c:v>ZM</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
           </c:cat>
           <c:val>
             <c:numRef>
@@ -875,7 +1596,20 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-2045-4D73-BC02-AB081A338646}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
         <c:gapWidth val="2"/>
         <c:axId val="50010001"/>
         <c:axId val="50010002"/>
@@ -885,23 +1619,30 @@
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="50010002"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
         <c:axId val="50010002"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="50010001"/>
         <c:crosses val="autoZero"/>
@@ -910,9 +1651,11 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
+      <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
@@ -923,91 +1666,147 @@
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
   <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:barChart>
         <c:barDir val="col"/>
         <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
+          <c:invertIfNegative val="0"/>
           <c:cat>
-            <c:strRef>
-              <c:f>Sheet2!$B$2:$B$125</c:f>
-              <c:strCache>
-                <c:ptCount val="124"/>
-                <c:pt idx="0">
-                  <c:v>ACB 12/11 7p</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>CRSR 12/18 45C</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>F 12/4 10c</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>FB 12/18 300c</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>FB 12/4 290C</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>FSLY 12/4 90C</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>GME 12/18 20C</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>NKLA 12/31 20P</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>NKLA 12/4 17p</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>PLTR 1/15 40c</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>PLTR 12/31 32c</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>PLTR 12/31 35C</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>PLTR 12/4 35c</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>PLTR 12/4 38c</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>SLV 12/18 25c</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>SNOW 12/18 365c</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>SPY 12/4 362p</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>TSLA 12/11 600c</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>TSLA 12/4 650c</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>TSM 1/21 80c</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+            <c:multiLvlStrRef>
+              <c:f>Sheet2!$A$2:$B$21</c:f>
+              <c:multiLvlStrCache>
+                <c:ptCount val="20"/>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>12/11 7p</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>12/18 45C</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>12/4 10c</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>12/18 300c</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>12/4 290C</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>12/4 90C</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>12/18 20C</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>12/31 20P</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>12/4 17p</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>1/15 40c</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>12/31 32c</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
+                    <c:v>12/31 35C</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>12/4 35c</c:v>
+                  </c:pt>
+                  <c:pt idx="13">
+                    <c:v>12/4 38c</c:v>
+                  </c:pt>
+                  <c:pt idx="14">
+                    <c:v>12/18 25c</c:v>
+                  </c:pt>
+                  <c:pt idx="15">
+                    <c:v>12/18 365c</c:v>
+                  </c:pt>
+                  <c:pt idx="16">
+                    <c:v>12/4 362p</c:v>
+                  </c:pt>
+                  <c:pt idx="17">
+                    <c:v>12/11 600c</c:v>
+                  </c:pt>
+                  <c:pt idx="18">
+                    <c:v>12/4 650c</c:v>
+                  </c:pt>
+                  <c:pt idx="19">
+                    <c:v>1/21 80c</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>ACB</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>CRSR</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>F</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>FB</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>FSLY</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>GME</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>NKLA</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>PLTR</c:v>
+                  </c:pt>
+                  <c:pt idx="14">
+                    <c:v>SLV</c:v>
+                  </c:pt>
+                  <c:pt idx="15">
+                    <c:v>SNOW</c:v>
+                  </c:pt>
+                  <c:pt idx="16">
+                    <c:v>SPY</c:v>
+                  </c:pt>
+                  <c:pt idx="17">
+                    <c:v>TSLA</c:v>
+                  </c:pt>
+                  <c:pt idx="19">
+                    <c:v>TSM</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet2!$C$3:$C$125</c:f>
+              <c:f>Sheet2!$C$3:$C$21</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="123"/>
+                <c:ptCount val="19"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -1068,7 +1867,20 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-E562-4C1A-9D81-275F023E7925}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
         <c:gapWidth val="2"/>
         <c:axId val="50020001"/>
         <c:axId val="50020002"/>
@@ -1078,22 +1890,30 @@
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="50020002"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
         <c:axId val="50020002"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="50020001"/>
         <c:crosses val="autoZero"/>
@@ -1102,9 +1922,11 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
+      <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
@@ -1131,7 +1953,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -1153,20 +1981,26 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>609599</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>542925</xdr:colOff>
       <xdr:row>15</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -1227,7 +2061,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1259,9 +2093,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1293,6 +2145,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1468,14 +2338,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C125"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -1486,8 +2356,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -1497,8 +2367,8 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
-      <c r="A3" s="1"/>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3" s="2"/>
       <c r="B3" s="1" t="s">
         <v>107</v>
       </c>
@@ -1506,8 +2376,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
-      <c r="A4" s="1" t="s">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
@@ -1517,8 +2387,8 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
-      <c r="A5" s="1"/>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A5" s="2"/>
       <c r="B5" s="1" t="s">
         <v>107</v>
       </c>
@@ -1526,7 +2396,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
@@ -1537,7 +2407,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
@@ -1548,7 +2418,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
@@ -1559,7 +2429,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
@@ -1570,7 +2440,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
@@ -1581,7 +2451,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
@@ -1592,7 +2462,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
@@ -1603,7 +2473,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
@@ -1614,7 +2484,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
@@ -1625,7 +2495,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
         <v>13</v>
       </c>
@@ -1636,7 +2506,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
         <v>14</v>
       </c>
@@ -1647,7 +2517,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
         <v>15</v>
       </c>
@@ -1658,8 +2528,8 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:3">
-      <c r="A18" s="1" t="s">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A18" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B18" s="1" t="s">
@@ -1669,8 +2539,8 @@
         <v>25</v>
       </c>
     </row>
-    <row r="19" spans="1:3">
-      <c r="A19" s="1"/>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A19" s="2"/>
       <c r="B19" s="1" t="s">
         <v>107</v>
       </c>
@@ -1678,7 +2548,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="20" spans="1:3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
         <v>17</v>
       </c>
@@ -1689,7 +2559,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
         <v>18</v>
       </c>
@@ -1700,7 +2570,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
         <v>19</v>
       </c>
@@ -1711,7 +2581,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
         <v>20</v>
       </c>
@@ -1722,7 +2592,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
         <v>21</v>
       </c>
@@ -1733,7 +2603,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="s">
         <v>22</v>
       </c>
@@ -1744,7 +2614,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="s">
         <v>23</v>
       </c>
@@ -1755,7 +2625,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="27" spans="1:3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A27" s="1" t="s">
         <v>24</v>
       </c>
@@ -1766,7 +2636,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A28" s="1" t="s">
         <v>25</v>
       </c>
@@ -1777,7 +2647,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A29" s="1" t="s">
         <v>26</v>
       </c>
@@ -1788,8 +2658,8 @@
         <v>3</v>
       </c>
     </row>
-    <row r="30" spans="1:3">
-      <c r="A30" s="1" t="s">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A30" s="2" t="s">
         <v>27</v>
       </c>
       <c r="B30" s="1" t="s">
@@ -1799,8 +2669,8 @@
         <v>5</v>
       </c>
     </row>
-    <row r="31" spans="1:3">
-      <c r="A31" s="1"/>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A31" s="2"/>
       <c r="B31" s="1" t="s">
         <v>107</v>
       </c>
@@ -1808,7 +2678,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:3">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A32" s="1" t="s">
         <v>28</v>
       </c>
@@ -1819,7 +2689,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:3">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A33" s="1" t="s">
         <v>29</v>
       </c>
@@ -1830,7 +2700,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:3">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A34" s="1" t="s">
         <v>30</v>
       </c>
@@ -1841,7 +2711,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:3">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A35" s="1" t="s">
         <v>31</v>
       </c>
@@ -1852,7 +2722,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:3">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A36" s="1" t="s">
         <v>32</v>
       </c>
@@ -1863,8 +2733,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="37" spans="1:3">
-      <c r="A37" s="1" t="s">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A37" s="2" t="s">
         <v>33</v>
       </c>
       <c r="B37" s="1" t="s">
@@ -1874,8 +2744,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:3">
-      <c r="A38" s="1"/>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A38" s="2"/>
       <c r="B38" s="1" t="s">
         <v>107</v>
       </c>
@@ -1883,7 +2753,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:3">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A39" s="1" t="s">
         <v>34</v>
       </c>
@@ -1894,7 +2764,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:3">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A40" s="1" t="s">
         <v>35</v>
       </c>
@@ -1905,7 +2775,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:3">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A41" s="1" t="s">
         <v>36</v>
       </c>
@@ -1916,8 +2786,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:3">
-      <c r="A42" s="1" t="s">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A42" s="2" t="s">
         <v>37</v>
       </c>
       <c r="B42" s="1" t="s">
@@ -1927,8 +2797,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:3">
-      <c r="A43" s="1"/>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A43" s="2"/>
       <c r="B43" s="1" t="s">
         <v>107</v>
       </c>
@@ -1936,8 +2806,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:3">
-      <c r="A44" s="1" t="s">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A44" s="2" t="s">
         <v>38</v>
       </c>
       <c r="B44" s="1" t="s">
@@ -1947,8 +2817,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="45" spans="1:3">
-      <c r="A45" s="1"/>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A45" s="2"/>
       <c r="B45" s="1" t="s">
         <v>107</v>
       </c>
@@ -1956,7 +2826,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:3">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A46" s="1" t="s">
         <v>39</v>
       </c>
@@ -1967,7 +2837,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="47" spans="1:3">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A47" s="1" t="s">
         <v>40</v>
       </c>
@@ -1978,7 +2848,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:3">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A48" s="1" t="s">
         <v>41</v>
       </c>
@@ -1989,8 +2859,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:3">
-      <c r="A49" s="1" t="s">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A49" s="2" t="s">
         <v>42</v>
       </c>
       <c r="B49" s="1" t="s">
@@ -2000,8 +2870,8 @@
         <v>15</v>
       </c>
     </row>
-    <row r="50" spans="1:3">
-      <c r="A50" s="1"/>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A50" s="2"/>
       <c r="B50" s="1" t="s">
         <v>107</v>
       </c>
@@ -2009,7 +2879,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="51" spans="1:3">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A51" s="1" t="s">
         <v>43</v>
       </c>
@@ -2020,7 +2890,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:3">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A52" s="1" t="s">
         <v>44</v>
       </c>
@@ -2031,8 +2901,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="53" spans="1:3">
-      <c r="A53" s="1" t="s">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A53" s="2" t="s">
         <v>45</v>
       </c>
       <c r="B53" s="1" t="s">
@@ -2042,8 +2912,8 @@
         <v>8</v>
       </c>
     </row>
-    <row r="54" spans="1:3">
-      <c r="A54" s="1"/>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A54" s="2"/>
       <c r="B54" s="1" t="s">
         <v>107</v>
       </c>
@@ -2051,7 +2921,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="55" spans="1:3">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A55" s="1" t="s">
         <v>46</v>
       </c>
@@ -2062,8 +2932,8 @@
         <v>3</v>
       </c>
     </row>
-    <row r="56" spans="1:3">
-      <c r="A56" s="1" t="s">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A56" s="2" t="s">
         <v>47</v>
       </c>
       <c r="B56" s="1" t="s">
@@ -2073,8 +2943,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="57" spans="1:3">
-      <c r="A57" s="1"/>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A57" s="2"/>
       <c r="B57" s="1" t="s">
         <v>107</v>
       </c>
@@ -2082,8 +2952,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:3">
-      <c r="A58" s="1" t="s">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A58" s="2" t="s">
         <v>48</v>
       </c>
       <c r="B58" s="1" t="s">
@@ -2093,8 +2963,8 @@
         <v>4</v>
       </c>
     </row>
-    <row r="59" spans="1:3">
-      <c r="A59" s="1"/>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A59" s="2"/>
       <c r="B59" s="1" t="s">
         <v>107</v>
       </c>
@@ -2102,7 +2972,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="60" spans="1:3">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A60" s="1" t="s">
         <v>49</v>
       </c>
@@ -2113,8 +2983,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:3">
-      <c r="A61" s="1" t="s">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A61" s="2" t="s">
         <v>50</v>
       </c>
       <c r="B61" s="1" t="s">
@@ -2124,8 +2994,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="1:3">
-      <c r="A62" s="1"/>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A62" s="2"/>
       <c r="B62" s="1" t="s">
         <v>107</v>
       </c>
@@ -2133,7 +3003,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:3">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A63" s="1" t="s">
         <v>51</v>
       </c>
@@ -2144,7 +3014,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="1:3">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A64" s="1" t="s">
         <v>52</v>
       </c>
@@ -2155,7 +3025,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="1:3">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A65" s="1" t="s">
         <v>53</v>
       </c>
@@ -2166,7 +3036,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:3">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A66" s="1" t="s">
         <v>54</v>
       </c>
@@ -2177,7 +3047,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="1:3">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A67" s="1" t="s">
         <v>55</v>
       </c>
@@ -2188,7 +3058,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="1:3">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A68" s="1" t="s">
         <v>56</v>
       </c>
@@ -2199,8 +3069,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="69" spans="1:3">
-      <c r="A69" s="1" t="s">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A69" s="2" t="s">
         <v>57</v>
       </c>
       <c r="B69" s="1" t="s">
@@ -2210,8 +3080,8 @@
         <v>8</v>
       </c>
     </row>
-    <row r="70" spans="1:3">
-      <c r="A70" s="1"/>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A70" s="2"/>
       <c r="B70" s="1" t="s">
         <v>107</v>
       </c>
@@ -2219,7 +3089,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="71" spans="1:3">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A71" s="1" t="s">
         <v>58</v>
       </c>
@@ -2230,7 +3100,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="72" spans="1:3">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A72" s="1" t="s">
         <v>59</v>
       </c>
@@ -2241,7 +3111,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="73" spans="1:3">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A73" s="1" t="s">
         <v>60</v>
       </c>
@@ -2252,8 +3122,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="74" spans="1:3">
-      <c r="A74" s="1" t="s">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A74" s="2" t="s">
         <v>61</v>
       </c>
       <c r="B74" s="1" t="s">
@@ -2263,8 +3133,8 @@
         <v>9</v>
       </c>
     </row>
-    <row r="75" spans="1:3">
-      <c r="A75" s="1"/>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A75" s="2"/>
       <c r="B75" s="1" t="s">
         <v>107</v>
       </c>
@@ -2272,8 +3142,8 @@
         <v>6</v>
       </c>
     </row>
-    <row r="76" spans="1:3">
-      <c r="A76" s="1" t="s">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A76" s="2" t="s">
         <v>62</v>
       </c>
       <c r="B76" s="1" t="s">
@@ -2283,8 +3153,8 @@
         <v>9</v>
       </c>
     </row>
-    <row r="77" spans="1:3">
-      <c r="A77" s="1"/>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A77" s="2"/>
       <c r="B77" s="1" t="s">
         <v>107</v>
       </c>
@@ -2292,7 +3162,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="78" spans="1:3">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A78" s="1" t="s">
         <v>63</v>
       </c>
@@ -2303,8 +3173,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="79" spans="1:3">
-      <c r="A79" s="1" t="s">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A79" s="2" t="s">
         <v>64</v>
       </c>
       <c r="B79" s="1" t="s">
@@ -2314,8 +3184,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="80" spans="1:3">
-      <c r="A80" s="1"/>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A80" s="2"/>
       <c r="B80" s="1" t="s">
         <v>107</v>
       </c>
@@ -2323,7 +3193,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="81" spans="1:3">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A81" s="1" t="s">
         <v>65</v>
       </c>
@@ -2334,8 +3204,8 @@
         <v>9</v>
       </c>
     </row>
-    <row r="82" spans="1:3">
-      <c r="A82" s="1" t="s">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A82" s="2" t="s">
         <v>66</v>
       </c>
       <c r="B82" s="1" t="s">
@@ -2345,8 +3215,8 @@
         <v>51</v>
       </c>
     </row>
-    <row r="83" spans="1:3">
-      <c r="A83" s="1"/>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A83" s="2"/>
       <c r="B83" s="1" t="s">
         <v>107</v>
       </c>
@@ -2354,7 +3224,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="84" spans="1:3">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A84" s="1" t="s">
         <v>67</v>
       </c>
@@ -2365,7 +3235,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="85" spans="1:3">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A85" s="1" t="s">
         <v>68</v>
       </c>
@@ -2376,7 +3246,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="86" spans="1:3">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A86" s="1" t="s">
         <v>69</v>
       </c>
@@ -2387,7 +3257,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="87" spans="1:3">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A87" s="1" t="s">
         <v>70</v>
       </c>
@@ -2398,7 +3268,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="88" spans="1:3">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A88" s="1" t="s">
         <v>71</v>
       </c>
@@ -2409,7 +3279,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="89" spans="1:3">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A89" s="1" t="s">
         <v>72</v>
       </c>
@@ -2420,7 +3290,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="90" spans="1:3">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A90" s="1" t="s">
         <v>73</v>
       </c>
@@ -2431,7 +3301,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="91" spans="1:3">
+    <row r="91" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A91" s="1" t="s">
         <v>74</v>
       </c>
@@ -2442,7 +3312,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="92" spans="1:3">
+    <row r="92" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A92" s="1" t="s">
         <v>75</v>
       </c>
@@ -2453,7 +3323,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="93" spans="1:3">
+    <row r="93" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A93" s="1" t="s">
         <v>76</v>
       </c>
@@ -2464,7 +3334,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="94" spans="1:3">
+    <row r="94" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A94" s="1" t="s">
         <v>77</v>
       </c>
@@ -2475,7 +3345,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="95" spans="1:3">
+    <row r="95" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A95" s="1" t="s">
         <v>78</v>
       </c>
@@ -2486,7 +3356,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="96" spans="1:3">
+    <row r="96" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A96" s="1" t="s">
         <v>79</v>
       </c>
@@ -2497,7 +3367,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="97" spans="1:3">
+    <row r="97" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A97" s="1" t="s">
         <v>80</v>
       </c>
@@ -2508,7 +3378,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="98" spans="1:3">
+    <row r="98" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A98" s="1" t="s">
         <v>81</v>
       </c>
@@ -2519,7 +3389,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="99" spans="1:3">
+    <row r="99" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A99" s="1" t="s">
         <v>82</v>
       </c>
@@ -2530,8 +3400,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="100" spans="1:3">
-      <c r="A100" s="1" t="s">
+    <row r="100" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A100" s="2" t="s">
         <v>83</v>
       </c>
       <c r="B100" s="1" t="s">
@@ -2541,8 +3411,8 @@
         <v>12</v>
       </c>
     </row>
-    <row r="101" spans="1:3">
-      <c r="A101" s="1"/>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A101" s="2"/>
       <c r="B101" s="1" t="s">
         <v>107</v>
       </c>
@@ -2550,7 +3420,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="102" spans="1:3">
+    <row r="102" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A102" s="1" t="s">
         <v>84</v>
       </c>
@@ -2561,7 +3431,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="103" spans="1:3">
+    <row r="103" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A103" s="1" t="s">
         <v>85</v>
       </c>
@@ -2572,7 +3442,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="104" spans="1:3">
+    <row r="104" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A104" s="1" t="s">
         <v>86</v>
       </c>
@@ -2583,7 +3453,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="105" spans="1:3">
+    <row r="105" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A105" s="1" t="s">
         <v>87</v>
       </c>
@@ -2594,8 +3464,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="106" spans="1:3">
-      <c r="A106" s="1" t="s">
+    <row r="106" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A106" s="2" t="s">
         <v>88</v>
       </c>
       <c r="B106" s="1" t="s">
@@ -2605,8 +3475,8 @@
         <v>26</v>
       </c>
     </row>
-    <row r="107" spans="1:3">
-      <c r="A107" s="1"/>
+    <row r="107" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A107" s="2"/>
       <c r="B107" s="1" t="s">
         <v>107</v>
       </c>
@@ -2614,7 +3484,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="108" spans="1:3">
+    <row r="108" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A108" s="1" t="s">
         <v>89</v>
       </c>
@@ -2625,7 +3495,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="109" spans="1:3">
+    <row r="109" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A109" s="1" t="s">
         <v>90</v>
       </c>
@@ -2636,7 +3506,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="110" spans="1:3">
+    <row r="110" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A110" s="1" t="s">
         <v>91</v>
       </c>
@@ -2647,7 +3517,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="111" spans="1:3">
+    <row r="111" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A111" s="1" t="s">
         <v>92</v>
       </c>
@@ -2658,7 +3528,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="112" spans="1:3">
+    <row r="112" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A112" s="1" t="s">
         <v>93</v>
       </c>
@@ -2669,7 +3539,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="113" spans="1:3">
+    <row r="113" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A113" s="1" t="s">
         <v>94</v>
       </c>
@@ -2680,7 +3550,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="114" spans="1:3">
+    <row r="114" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A114" s="1" t="s">
         <v>95</v>
       </c>
@@ -2691,7 +3561,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="115" spans="1:3">
+    <row r="115" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A115" s="1" t="s">
         <v>96</v>
       </c>
@@ -2702,7 +3572,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="116" spans="1:3">
+    <row r="116" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A116" s="1" t="s">
         <v>97</v>
       </c>
@@ -2713,7 +3583,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="117" spans="1:3">
+    <row r="117" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A117" s="1" t="s">
         <v>98</v>
       </c>
@@ -2724,7 +3594,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="118" spans="1:3">
+    <row r="118" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A118" s="1" t="s">
         <v>99</v>
       </c>
@@ -2735,7 +3605,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="119" spans="1:3">
+    <row r="119" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A119" s="1" t="s">
         <v>100</v>
       </c>
@@ -2746,7 +3616,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="120" spans="1:3">
+    <row r="120" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A120" s="1" t="s">
         <v>101</v>
       </c>
@@ -2757,7 +3627,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="121" spans="1:3">
+    <row r="121" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A121" s="1" t="s">
         <v>102</v>
       </c>
@@ -2768,7 +3638,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="122" spans="1:3">
+    <row r="122" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A122" s="1" t="s">
         <v>103</v>
       </c>
@@ -2779,7 +3649,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="123" spans="1:3">
+    <row r="123" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A123" s="1" t="s">
         <v>104</v>
       </c>
@@ -2790,8 +3660,8 @@
         <v>3</v>
       </c>
     </row>
-    <row r="124" spans="1:3">
-      <c r="A124" s="1" t="s">
+    <row r="124" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A124" s="2" t="s">
         <v>105</v>
       </c>
       <c r="B124" s="1" t="s">
@@ -2801,8 +3671,8 @@
         <v>12</v>
       </c>
     </row>
-    <row r="125" spans="1:3">
-      <c r="A125" s="1"/>
+    <row r="125" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A125" s="2"/>
       <c r="B125" s="1" t="s">
         <v>107</v>
       </c>
@@ -2812,26 +3682,26 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="A79:A80"/>
+    <mergeCell ref="A82:A83"/>
+    <mergeCell ref="A100:A101"/>
+    <mergeCell ref="A106:A107"/>
+    <mergeCell ref="A124:A125"/>
+    <mergeCell ref="A58:A59"/>
+    <mergeCell ref="A61:A62"/>
+    <mergeCell ref="A69:A70"/>
+    <mergeCell ref="A74:A75"/>
+    <mergeCell ref="A76:A77"/>
+    <mergeCell ref="A42:A43"/>
+    <mergeCell ref="A44:A45"/>
+    <mergeCell ref="A49:A50"/>
+    <mergeCell ref="A53:A54"/>
+    <mergeCell ref="A56:A57"/>
     <mergeCell ref="A2:A3"/>
     <mergeCell ref="A4:A5"/>
     <mergeCell ref="A18:A19"/>
     <mergeCell ref="A30:A31"/>
     <mergeCell ref="A37:A38"/>
-    <mergeCell ref="A42:A43"/>
-    <mergeCell ref="A44:A45"/>
-    <mergeCell ref="A49:A50"/>
-    <mergeCell ref="A53:A54"/>
-    <mergeCell ref="A56:A57"/>
-    <mergeCell ref="A58:A59"/>
-    <mergeCell ref="A61:A62"/>
-    <mergeCell ref="A69:A70"/>
-    <mergeCell ref="A74:A75"/>
-    <mergeCell ref="A76:A77"/>
-    <mergeCell ref="A79:A80"/>
-    <mergeCell ref="A82:A83"/>
-    <mergeCell ref="A100:A101"/>
-    <mergeCell ref="A106:A107"/>
-    <mergeCell ref="A124:A125"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -2839,14 +3709,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C21"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -2857,7 +3727,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
@@ -2868,7 +3738,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>27</v>
       </c>
@@ -2879,7 +3749,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>108</v>
       </c>
@@ -2890,8 +3760,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
-      <c r="A5" s="1" t="s">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A5" s="2" t="s">
         <v>37</v>
       </c>
       <c r="B5" s="1" t="s">
@@ -2901,8 +3771,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
-      <c r="A6" s="1"/>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A6" s="2"/>
       <c r="B6" s="1" t="s">
         <v>114</v>
       </c>
@@ -2910,7 +3780,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>109</v>
       </c>
@@ -2921,7 +3791,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>42</v>
       </c>
@@ -2932,8 +3802,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
-      <c r="A9" s="1" t="s">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A9" s="2" t="s">
         <v>62</v>
       </c>
       <c r="B9" s="1" t="s">
@@ -2943,8 +3813,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
-      <c r="A10" s="1"/>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A10" s="2"/>
       <c r="B10" s="1" t="s">
         <v>118</v>
       </c>
@@ -2952,8 +3822,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
-      <c r="A11" s="1" t="s">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A11" s="2" t="s">
         <v>66</v>
       </c>
       <c r="B11" s="1" t="s">
@@ -2963,8 +3833,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
-      <c r="A12" s="1"/>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A12" s="2"/>
       <c r="B12" s="1" t="s">
         <v>120</v>
       </c>
@@ -2972,8 +3842,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
-      <c r="A13" s="1"/>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A13" s="2"/>
       <c r="B13" s="1" t="s">
         <v>121</v>
       </c>
@@ -2981,8 +3851,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
-      <c r="A14" s="1"/>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A14" s="2"/>
       <c r="B14" s="1" t="s">
         <v>122</v>
       </c>
@@ -2990,8 +3860,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:3">
-      <c r="A15" s="1"/>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A15" s="2"/>
       <c r="B15" s="1" t="s">
         <v>123</v>
       </c>
@@ -2999,7 +3869,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
         <v>78</v>
       </c>
@@ -3010,7 +3880,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
         <v>80</v>
       </c>
@@ -3021,7 +3891,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
         <v>83</v>
       </c>
@@ -3032,8 +3902,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:3">
-      <c r="A19" s="1" t="s">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A19" s="2" t="s">
         <v>88</v>
       </c>
       <c r="B19" s="1" t="s">
@@ -3043,8 +3913,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:3">
-      <c r="A20" s="1"/>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A20" s="2"/>
       <c r="B20" s="1" t="s">
         <v>128</v>
       </c>
@@ -3052,7 +3922,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
         <v>89</v>
       </c>

</xml_diff>